<commit_message>
Alteração da Estrutura do padrão do projeto
</commit_message>
<xml_diff>
--- a/Metas.xlsx
+++ b/Metas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Funcionalidade</t>
   </si>
@@ -248,13 +248,19 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta a Tabela de Gestão do consumidor </t>
+  </si>
+  <si>
+    <t>Restante pro item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,14 +271,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +361,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -379,17 +383,17 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="7" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,12 +710,13 @@
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,9 +726,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -731,10 +738,13 @@
         <v>200</v>
       </c>
       <c r="C2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -745,7 +755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -756,7 +766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -767,7 +777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -778,7 +788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -789,7 +799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -800,7 +810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -810,19 +820,19 @@
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="4">
+      <c r="F9" s="3">
         <f>SUM(B2:B80)</f>
         <v>1957</v>
       </c>
-      <c r="H9" s="5">
+      <c r="G9" s="4">
         <f>SUM(C2:C80)</f>
-        <v>1428</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -833,7 +843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -843,16 +853,16 @@
       <c r="C11">
         <v>13</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="11">
-        <f>(H9/G9)*100%</f>
-        <v>0.72968829841594274</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="10">
+        <f>(G9/F9)*100%</f>
+        <v>0.71844660194174759</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -863,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -873,18 +883,18 @@
       <c r="C13">
         <v>8</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="10">
-        <f>(H9*20)/60</f>
-        <v>476</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="F13" s="9">
+        <f>(G9*20)/60</f>
+        <v>468.66666666666669</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -895,7 +905,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -906,7 +916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -917,7 +927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -927,11 +937,11 @@
       <c r="C17">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -942,7 +952,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -953,7 +963,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -964,7 +974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -975,7 +985,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -985,11 +995,11 @@
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1011,7 +1021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1022,7 +1032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1033,7 +1043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1044,7 +1054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1055,7 +1065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1066,7 +1076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1077,7 +1087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1088,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1529,9 +1539,9 @@
       </c>
     </row>
     <row r="82" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A82" s="3"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
+      <c r="A82" s="2"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>